<commit_message>
Mas datos para el excel. tocará comprobar que falla y que está guay.... engaaaa a por los verdes!!
</commit_message>
<xml_diff>
--- a/Otras cosas/Pronósticos-tenis/Datos.xlsx
+++ b/Otras cosas/Pronósticos-tenis/Datos.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2088" uniqueCount="988">
   <si>
     <t>ATP Halle</t>
   </si>
@@ -2446,6 +2447,540 @@
   </si>
   <si>
     <t>//----------Prob OVER/UNDER de 36.5 -&gt;&gt; ,40% - 99,60%</t>
+  </si>
+  <si>
+    <t>Robin Haase vs Roberto Bautista Agut</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador LOCAL: 164</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador VISITANTE: 836</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA LOCAL: 16,40%</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA VISITANTE: 83,60%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-0: 6,00%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-1: 10,40%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 0-2: 54,90%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 1-2: 28,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 14.5 -&gt;&gt; 99,40% - ,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 15.5 -&gt;&gt; 97,10% - 2,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 16.5 -&gt;&gt; 94,00% - 6,00%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 17.5 -&gt;&gt; 88,40% - 11,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 18.5 -&gt;&gt; 78,80% - 21,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 19.5 -&gt;&gt; 71,60% - 28,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 20.5 -&gt;&gt; 63,40% - 36,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 21.5 -&gt;&gt; 57,60% - 42,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 22.5 -&gt;&gt; 49,60% - 50,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 24.5 -&gt;&gt; 41,80% - 58,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 25.5 -&gt;&gt; 38,00% - 62,00%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 26.5 -&gt;&gt; 33,50% - 66,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 27.5 -&gt;&gt; 31,30% - 68,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 28.5 -&gt;&gt; 27,20% - 72,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 29.5 -&gt;&gt; 23,60% - 76,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 30.5 -&gt;&gt; 18,50% - 81,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 32.5 -&gt;&gt; 9,00% - 91,00%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 34.5 -&gt;&gt; 4,10% - 95,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 36.5 -&gt;&gt; ,80% - 99,20%</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador LOCAL: 814</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador VISITANTE: 186</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA LOCAL: 81,40%</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA VISITANTE: 18,60%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-0: 51,20%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 0-2: 7,80%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 1-2: 10,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 16.5 -&gt;&gt; 95,30% - 4,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 17.5 -&gt;&gt; 89,90% - 10,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 18.5 -&gt;&gt; 81,10% - 18,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 19.5 -&gt;&gt; 73,30% - 26,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 20.5 -&gt;&gt; 65,10% - 34,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 22.5 -&gt;&gt; 51,90% - 48,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 23.5 -&gt;&gt; 45,30% - 54,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 24.5 -&gt;&gt; 43,60% - 56,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 25.5 -&gt;&gt; 38,40% - 61,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 26.5 -&gt;&gt; 35,00% - 65,00%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 27.5 -&gt;&gt; 31,70% - 68,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 28.5 -&gt;&gt; 27,90% - 72,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 29.5 -&gt;&gt; 24,40% - 75,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 30.5 -&gt;&gt; 19,60% - 80,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 31.5 -&gt;&gt; 14,30% - 85,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 32.5 -&gt;&gt; 9,40% - 90,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 33.5 -&gt;&gt; 6,80% - 93,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 34.5 -&gt;&gt; 4,70% - 95,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 35.5 -&gt;&gt; 2,10% - 97,90%</t>
+  </si>
+  <si>
+    <t>Kei Nishikori vs Karen Khachanov</t>
+  </si>
+  <si>
+    <t>2-6 2-6 0-0</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 14.5 -&gt;&gt; 98,10% - 1,90%</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador LOCAL: 124</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador VISITANTE: 876</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA LOCAL: 12,40%</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA VISITANTE: 87,60%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-1: 7,70%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 0-2: 59,70%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 1-2: 27,90%</t>
+  </si>
+  <si>
+    <t>4-6 5-7 0-0</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 13.5 -&gt;&gt; 99,60% - ,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 15.5 -&gt;&gt; 97,70% - 2,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 16.5 -&gt;&gt; 93,30% - 6,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 17.5 -&gt;&gt; 87,10% - 12,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 18.5 -&gt;&gt; 76,70% - 23,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 19.5 -&gt;&gt; 68,40% - 31,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 20.5 -&gt;&gt; 60,30% - 39,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 21.5 -&gt;&gt; 54,30% - 45,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 22.5 -&gt;&gt; 46,50% - 53,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 23.5 -&gt;&gt; 40,10% - 59,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 24.5 -&gt;&gt; 38,80% - 61,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 25.5 -&gt;&gt; 35,90% - 64,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 26.5 -&gt;&gt; 31,60% - 68,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 27.5 -&gt;&gt; 28,30% - 71,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 28.5 -&gt;&gt; 24,70% - 75,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 29.5 -&gt;&gt; 21,40% - 78,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 30.5 -&gt;&gt; 18,10% - 81,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 31.5 -&gt;&gt; 13,90% - 86,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 32.5 -&gt;&gt; 9,60% - 90,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 34.5 -&gt;&gt; 5,10% - 94,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 35.5 -&gt;&gt; 2,20% - 97,80%</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador LOCAL: 698</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador VISITANTE: 302</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA LOCAL: 69,80%</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA VISITANTE: 30,20%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-0: 40,50%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-1: 29,30%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 0-2: 13,70%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 1-2: 16,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 15.5 -&gt;&gt; 98,90% - 1,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 17.5 -&gt;&gt; 94,20% - 5,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 18.5 -&gt;&gt; 89,20% - 10,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 20.5 -&gt;&gt; 73,40% - 26,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 22.5 -&gt;&gt; 60,10% - 39,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 23.5 -&gt;&gt; 53,10% - 46,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 24.5 -&gt;&gt; 52,40% - 47,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 26.5 -&gt;&gt; 42,00% - 58,00%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 27.5 -&gt;&gt; 39,20% - 60,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 28.5 -&gt;&gt; 34,80% - 65,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 29.5 -&gt;&gt; 30,90% - 69,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 30.5 -&gt;&gt; 26,70% - 73,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 31.5 -&gt;&gt; 19,40% - 80,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 32.5 -&gt;&gt; 13,70% - 86,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 33.5 -&gt;&gt; 10,40% - 89,60%</t>
+  </si>
+  <si>
+    <t>Dominic Thiem vs Yuichi Sugita</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador LOCAL: 13</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador VISITANTE: 987</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA LOCAL: 1,30%</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA VISITANTE: 98,70%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-0: ,40%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-1: ,90%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 0-2: 86,50%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 1-2: 12,20%</t>
+  </si>
+  <si>
+    <t>///PROBABILIDAD:  10,20%</t>
+  </si>
+  <si>
+    <t>///PROBABILIDAD:  6,40%</t>
+  </si>
+  <si>
+    <t>///PROBABILIDAD:  5,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 13.5 -&gt;&gt; 99,50% - ,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 15.5 -&gt;&gt; 94,30% - 5,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 16.5 -&gt;&gt; 86,50% - 13,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 17.5 -&gt;&gt; 76,90% - 23,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 18.5 -&gt;&gt; 59,60% - 40,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 19.5 -&gt;&gt; 51,50% - 48,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 20.5 -&gt;&gt; 37,30% - 62,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 21.5 -&gt;&gt; 30,60% - 69,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 22.5 -&gt;&gt; 21,50% - 78,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 23.5 -&gt;&gt; 15,40% - 84,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 24.5 -&gt;&gt; 14,70% - 85,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 25.5 -&gt;&gt; 13,30% - 86,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 26.5 -&gt;&gt; 11,00% - 89,00%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 27.5 -&gt;&gt; 10,10% - 89,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 28.5 -&gt;&gt; 8,80% - 91,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 29.5 -&gt;&gt; 7,60% - 92,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 30.5 -&gt;&gt; 5,70% - 94,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 31.5 -&gt;&gt; 4,30% - 95,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 32.5 -&gt;&gt; 3,10% - 96,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 33.5 -&gt;&gt; 1,80% - 98,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 34.5 -&gt;&gt; 1,40% - 98,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 35.5 -&gt;&gt; ,60% - 99,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 37.5 -&gt;&gt; ,20% - 99,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 38.5 -&gt;&gt; ,00% - 100,00%</t>
+  </si>
+  <si>
+    <t>Stan Wawrinka vs Sam Querrey</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador LOCAL: 804</t>
+  </si>
+  <si>
+    <t>//------Victorias del jugador VISITANTE: 196</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA LOCAL: 80,40%</t>
+  </si>
+  <si>
+    <t>//------PROBABILIDAD DE VICTORIA VISITANTE: 19,60%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-0: 51,90%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 2-1: 28,50%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 0-2: 7,20%</t>
+  </si>
+  <si>
+    <t>PROBABILIDAD DE UN 1-2: 12,40%</t>
+  </si>
+  <si>
+    <t>///PROBABILIDAD:  6,60%</t>
+  </si>
+  <si>
+    <t>6-2 6-3 0-0</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 17.5 -&gt;&gt; 92,30% - 7,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 18.5 -&gt;&gt; 86,50% - 13,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 19.5 -&gt;&gt; 79,20% - 20,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 20.5 -&gt;&gt; 69,20% - 30,80%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 21.5 -&gt;&gt; 64,50% - 35,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 22.5 -&gt;&gt; 54,60% - 45,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 23.5 -&gt;&gt; 46,60% - 53,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 24.5 -&gt;&gt; 45,60% - 54,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 25.5 -&gt;&gt; 42,30% - 57,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 26.5 -&gt;&gt; 37,30% - 62,70%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 27.5 -&gt;&gt; 35,40% - 64,60%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 28.5 -&gt;&gt; 32,80% - 67,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 29.5 -&gt;&gt; 29,60% - 70,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 30.5 -&gt;&gt; 23,60% - 76,40%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 31.5 -&gt;&gt; 18,50% - 81,50%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 32.5 -&gt;&gt; 13,90% - 86,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 33.5 -&gt;&gt; 10,70% - 89,30%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 34.5 -&gt;&gt; 8,80% - 91,20%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 36.5 -&gt;&gt; 2,10% - 97,90%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 37.5 -&gt;&gt; 1,90% - 98,10%</t>
+  </si>
+  <si>
+    <t>//----------Prob OVER/UNDER de 38.5 -&gt;&gt; 1,30% - 98,70%</t>
+  </si>
+  <si>
+    <t>Daniil Medvedev vs Jeremy Chardy</t>
   </si>
 </sst>
 </file>
@@ -3601,6 +4136,293 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4572000" y="190500"/>
+          <a:ext cx="10858500" cy="4886325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4572000" y="11649075"/>
+          <a:ext cx="10791825" cy="7058025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4572000" y="23088600"/>
+          <a:ext cx="10820400" cy="7658100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1028" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4572000" y="34156650"/>
+          <a:ext cx="10820400" cy="7181850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1029" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4572000" y="45605700"/>
+          <a:ext cx="10839450" cy="2971800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>298</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>335</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1030" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4572000" y="56864250"/>
+          <a:ext cx="10801350" cy="7162800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -12239,7 +13061,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:F420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A339" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A288" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G362" sqref="G362"/>
     </sheetView>
   </sheetViews>
@@ -16156,4 +16978,3343 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:F357"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B359" sqref="B359"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:6">
+      <c r="B2" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="4" t="s">
+        <v>811</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="4" t="s">
+        <v>812</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="4" t="s">
+        <v>813</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="4" t="s">
+        <v>814</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12" s="4" t="s">
+        <v>815</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" s="4" t="s">
+        <v>816</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" s="4" t="s">
+        <v>817</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="B15" s="4" t="s">
+        <v>818</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="B16" s="4"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="4"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="2:6">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="4" t="s">
+        <v>819</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="4" t="s">
+        <v>820</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="4" t="s">
+        <v>821</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="4" t="s">
+        <v>822</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="4" t="s">
+        <v>823</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="4" t="s">
+        <v>824</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="4" t="s">
+        <v>825</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="4" t="s">
+        <v>826</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="4" t="s">
+        <v>827</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="4" t="s">
+        <v>828</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="4" t="s">
+        <v>829</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="4" t="s">
+        <v>830</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="B47" s="4" t="s">
+        <v>831</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="B48" s="4" t="s">
+        <v>832</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="4" t="s">
+        <v>833</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="4" t="s">
+        <v>834</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="2:6">
+      <c r="B51" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="4" t="s">
+        <v>835</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="4" t="s">
+        <v>836</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="4" t="s">
+        <v>837</v>
+      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="2:6">
+      <c r="B59" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B60" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="62" spans="2:6">
+      <c r="B62" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="2:6">
+      <c r="B63" s="4"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="2:6">
+      <c r="B64" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="2:6">
+      <c r="B65" s="4" t="s">
+        <v>838</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="2:6">
+      <c r="B66" s="4" t="s">
+        <v>839</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="2:6">
+      <c r="B67" s="4" t="s">
+        <v>840</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="2:6">
+      <c r="B68" s="4" t="s">
+        <v>841</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="2:6">
+      <c r="B69" s="4"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="2:6">
+      <c r="B70" s="4"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="2:6">
+      <c r="B71" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="2:6">
+      <c r="B72" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="2:6">
+      <c r="B73" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+      <c r="E73" s="5"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="2:6">
+      <c r="B74" s="4" t="s">
+        <v>843</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+      <c r="E74" s="5"/>
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="2:6">
+      <c r="B75" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="2:6">
+      <c r="B76" s="4"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="2:6">
+      <c r="B77" s="4"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+      <c r="E77" s="5"/>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="2:6">
+      <c r="B78" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="2:6">
+      <c r="B79" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E79" s="5"/>
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="2:6">
+      <c r="B80" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E80" s="5"/>
+      <c r="F80" s="6"/>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E81" s="5"/>
+      <c r="F81" s="6"/>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="E82" s="5"/>
+      <c r="F82" s="6"/>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="5"/>
+      <c r="F83" s="6"/>
+    </row>
+    <row r="84" spans="2:6">
+      <c r="B84" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E84" s="5"/>
+      <c r="F84" s="6"/>
+    </row>
+    <row r="85" spans="2:6">
+      <c r="B85" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E85" s="5"/>
+      <c r="F85" s="6"/>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="B86" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E86" s="5"/>
+      <c r="F86" s="6"/>
+    </row>
+    <row r="87" spans="2:6">
+      <c r="B87" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E87" s="5"/>
+      <c r="F87" s="6"/>
+    </row>
+    <row r="88" spans="2:6">
+      <c r="B88" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" s="5"/>
+      <c r="F88" s="6"/>
+    </row>
+    <row r="89" spans="2:6">
+      <c r="B89" s="4"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+      <c r="E89" s="5"/>
+      <c r="F89" s="6"/>
+    </row>
+    <row r="90" spans="2:6">
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+      <c r="E90" s="5"/>
+      <c r="F90" s="6"/>
+    </row>
+    <row r="91" spans="2:6">
+      <c r="B91" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="6"/>
+    </row>
+    <row r="92" spans="2:6">
+      <c r="B92" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="6"/>
+    </row>
+    <row r="93" spans="2:6">
+      <c r="B93" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+      <c r="E93" s="5"/>
+      <c r="F93" s="6"/>
+    </row>
+    <row r="94" spans="2:6">
+      <c r="B94" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+      <c r="E94" s="5"/>
+      <c r="F94" s="6"/>
+    </row>
+    <row r="95" spans="2:6">
+      <c r="B95" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+      <c r="E95" s="5"/>
+      <c r="F95" s="6"/>
+    </row>
+    <row r="96" spans="2:6">
+      <c r="B96" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="6"/>
+    </row>
+    <row r="97" spans="2:6">
+      <c r="B97" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="C97" s="5"/>
+      <c r="D97" s="5"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="6"/>
+    </row>
+    <row r="98" spans="2:6">
+      <c r="B98" s="4" t="s">
+        <v>847</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="6"/>
+    </row>
+    <row r="99" spans="2:6">
+      <c r="B99" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="6"/>
+    </row>
+    <row r="100" spans="2:6">
+      <c r="B100" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+      <c r="E100" s="5"/>
+      <c r="F100" s="6"/>
+    </row>
+    <row r="101" spans="2:6">
+      <c r="B101" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5"/>
+      <c r="E101" s="5"/>
+      <c r="F101" s="6"/>
+    </row>
+    <row r="102" spans="2:6">
+      <c r="B102" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5"/>
+      <c r="E102" s="5"/>
+      <c r="F102" s="6"/>
+    </row>
+    <row r="103" spans="2:6">
+      <c r="B103" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="6"/>
+    </row>
+    <row r="104" spans="2:6">
+      <c r="B104" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="6"/>
+    </row>
+    <row r="105" spans="2:6">
+      <c r="B105" s="4" t="s">
+        <v>853</v>
+      </c>
+      <c r="C105" s="5"/>
+      <c r="D105" s="5"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="6"/>
+    </row>
+    <row r="106" spans="2:6">
+      <c r="B106" s="4" t="s">
+        <v>854</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="6"/>
+    </row>
+    <row r="107" spans="2:6">
+      <c r="B107" s="4" t="s">
+        <v>855</v>
+      </c>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="6"/>
+    </row>
+    <row r="108" spans="2:6">
+      <c r="B108" s="4" t="s">
+        <v>856</v>
+      </c>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+      <c r="E108" s="5"/>
+      <c r="F108" s="6"/>
+    </row>
+    <row r="109" spans="2:6">
+      <c r="B109" s="4" t="s">
+        <v>857</v>
+      </c>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+      <c r="F109" s="6"/>
+    </row>
+    <row r="110" spans="2:6">
+      <c r="B110" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+      <c r="E110" s="5"/>
+      <c r="F110" s="6"/>
+    </row>
+    <row r="111" spans="2:6">
+      <c r="B111" s="4" t="s">
+        <v>859</v>
+      </c>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="6"/>
+    </row>
+    <row r="112" spans="2:6">
+      <c r="B112" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="6"/>
+    </row>
+    <row r="113" spans="2:6">
+      <c r="B113" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="6"/>
+    </row>
+    <row r="114" spans="2:6">
+      <c r="B114" s="4" t="s">
+        <v>862</v>
+      </c>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="6"/>
+    </row>
+    <row r="115" spans="2:6">
+      <c r="B115" s="4" t="s">
+        <v>863</v>
+      </c>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="6"/>
+    </row>
+    <row r="116" spans="2:6">
+      <c r="B116" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+      <c r="F116" s="6"/>
+    </row>
+    <row r="117" spans="2:6">
+      <c r="B117" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+      <c r="F117" s="6"/>
+    </row>
+    <row r="118" spans="2:6">
+      <c r="B118" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+      <c r="F118" s="6"/>
+    </row>
+    <row r="119" spans="2:6">
+      <c r="B119" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="6"/>
+    </row>
+    <row r="120" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B120" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C120" s="8"/>
+      <c r="D120" s="8"/>
+      <c r="E120" s="8"/>
+      <c r="F120" s="9"/>
+    </row>
+    <row r="121" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="122" spans="2:6">
+      <c r="B122" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122" s="2"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="3"/>
+    </row>
+    <row r="123" spans="2:6">
+      <c r="B123" s="4" t="s">
+        <v>867</v>
+      </c>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="5"/>
+      <c r="F123" s="6"/>
+    </row>
+    <row r="124" spans="2:6">
+      <c r="B124" s="4" t="s">
+        <v>868</v>
+      </c>
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
+      <c r="F124" s="6"/>
+    </row>
+    <row r="125" spans="2:6">
+      <c r="B125" s="4" t="s">
+        <v>869</v>
+      </c>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="5"/>
+      <c r="F125" s="6"/>
+    </row>
+    <row r="126" spans="2:6">
+      <c r="B126" s="4" t="s">
+        <v>870</v>
+      </c>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="5"/>
+      <c r="F126" s="6"/>
+    </row>
+    <row r="127" spans="2:6">
+      <c r="B127" s="4"/>
+      <c r="C127" s="5"/>
+      <c r="D127" s="5"/>
+      <c r="E127" s="5"/>
+      <c r="F127" s="6"/>
+    </row>
+    <row r="128" spans="2:6">
+      <c r="B128" s="4"/>
+      <c r="C128" s="5"/>
+      <c r="D128" s="5"/>
+      <c r="E128" s="5"/>
+      <c r="F128" s="6"/>
+    </row>
+    <row r="129" spans="2:6">
+      <c r="B129" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129" s="5"/>
+      <c r="D129" s="5"/>
+      <c r="E129" s="5"/>
+      <c r="F129" s="6"/>
+    </row>
+    <row r="130" spans="2:6">
+      <c r="B130" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="C130" s="5"/>
+      <c r="D130" s="5"/>
+      <c r="E130" s="5"/>
+      <c r="F130" s="6"/>
+    </row>
+    <row r="131" spans="2:6">
+      <c r="B131" s="4" t="s">
+        <v>871</v>
+      </c>
+      <c r="C131" s="5"/>
+      <c r="D131" s="5"/>
+      <c r="E131" s="5"/>
+      <c r="F131" s="6"/>
+    </row>
+    <row r="132" spans="2:6">
+      <c r="B132" s="4" t="s">
+        <v>872</v>
+      </c>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="6"/>
+    </row>
+    <row r="133" spans="2:6">
+      <c r="B133" s="4" t="s">
+        <v>873</v>
+      </c>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="6"/>
+    </row>
+    <row r="134" spans="2:6">
+      <c r="B134" s="4"/>
+      <c r="C134" s="5"/>
+      <c r="D134" s="5"/>
+      <c r="E134" s="5"/>
+      <c r="F134" s="6"/>
+    </row>
+    <row r="135" spans="2:6">
+      <c r="B135" s="4"/>
+      <c r="C135" s="5"/>
+      <c r="D135" s="5"/>
+      <c r="E135" s="5"/>
+      <c r="F135" s="6"/>
+    </row>
+    <row r="136" spans="2:6">
+      <c r="B136" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+      <c r="E136" s="5"/>
+      <c r="F136" s="6"/>
+    </row>
+    <row r="137" spans="2:6">
+      <c r="B137" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C137" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D137" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E137" s="5"/>
+      <c r="F137" s="6"/>
+    </row>
+    <row r="138" spans="2:6">
+      <c r="B138" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D138" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E138" s="5"/>
+      <c r="F138" s="6"/>
+    </row>
+    <row r="139" spans="2:6">
+      <c r="B139" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E139" s="5"/>
+      <c r="F139" s="6"/>
+    </row>
+    <row r="140" spans="2:6">
+      <c r="B140" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E140" s="5"/>
+      <c r="F140" s="6"/>
+    </row>
+    <row r="141" spans="2:6">
+      <c r="B141" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D141" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E141" s="5"/>
+      <c r="F141" s="6"/>
+    </row>
+    <row r="142" spans="2:6">
+      <c r="B142" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D142" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E142" s="5"/>
+      <c r="F142" s="6"/>
+    </row>
+    <row r="143" spans="2:6">
+      <c r="B143" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C143" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E143" s="5"/>
+      <c r="F143" s="6"/>
+    </row>
+    <row r="144" spans="2:6">
+      <c r="B144" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C144" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E144" s="5"/>
+      <c r="F144" s="6"/>
+    </row>
+    <row r="145" spans="2:6">
+      <c r="B145" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>874</v>
+      </c>
+      <c r="E145" s="5"/>
+      <c r="F145" s="6"/>
+    </row>
+    <row r="146" spans="2:6">
+      <c r="B146" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E146" s="5"/>
+      <c r="F146" s="6"/>
+    </row>
+    <row r="147" spans="2:6">
+      <c r="B147" s="4"/>
+      <c r="C147" s="5"/>
+      <c r="D147" s="5"/>
+      <c r="E147" s="5"/>
+      <c r="F147" s="6"/>
+    </row>
+    <row r="148" spans="2:6">
+      <c r="B148" s="4"/>
+      <c r="C148" s="5"/>
+      <c r="D148" s="5"/>
+      <c r="E148" s="5"/>
+      <c r="F148" s="6"/>
+    </row>
+    <row r="149" spans="2:6">
+      <c r="B149" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C149" s="5"/>
+      <c r="D149" s="5"/>
+      <c r="E149" s="5"/>
+      <c r="F149" s="6"/>
+    </row>
+    <row r="150" spans="2:6">
+      <c r="B150" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="6"/>
+    </row>
+    <row r="151" spans="2:6">
+      <c r="B151" s="4" t="s">
+        <v>875</v>
+      </c>
+      <c r="C151" s="5"/>
+      <c r="D151" s="5"/>
+      <c r="E151" s="5"/>
+      <c r="F151" s="6"/>
+    </row>
+    <row r="152" spans="2:6">
+      <c r="B152" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="C152" s="5"/>
+      <c r="D152" s="5"/>
+      <c r="E152" s="5"/>
+      <c r="F152" s="6"/>
+    </row>
+    <row r="153" spans="2:6">
+      <c r="B153" s="4" t="s">
+        <v>876</v>
+      </c>
+      <c r="C153" s="5"/>
+      <c r="D153" s="5"/>
+      <c r="E153" s="5"/>
+      <c r="F153" s="6"/>
+    </row>
+    <row r="154" spans="2:6">
+      <c r="B154" s="4" t="s">
+        <v>877</v>
+      </c>
+      <c r="C154" s="5"/>
+      <c r="D154" s="5"/>
+      <c r="E154" s="5"/>
+      <c r="F154" s="6"/>
+    </row>
+    <row r="155" spans="2:6">
+      <c r="B155" s="4" t="s">
+        <v>878</v>
+      </c>
+      <c r="C155" s="5"/>
+      <c r="D155" s="5"/>
+      <c r="E155" s="5"/>
+      <c r="F155" s="6"/>
+    </row>
+    <row r="156" spans="2:6">
+      <c r="B156" s="4" t="s">
+        <v>879</v>
+      </c>
+      <c r="C156" s="5"/>
+      <c r="D156" s="5"/>
+      <c r="E156" s="5"/>
+      <c r="F156" s="6"/>
+    </row>
+    <row r="157" spans="2:6">
+      <c r="B157" s="4" t="s">
+        <v>880</v>
+      </c>
+      <c r="C157" s="5"/>
+      <c r="D157" s="5"/>
+      <c r="E157" s="5"/>
+      <c r="F157" s="6"/>
+    </row>
+    <row r="158" spans="2:6">
+      <c r="B158" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="C158" s="5"/>
+      <c r="D158" s="5"/>
+      <c r="E158" s="5"/>
+      <c r="F158" s="6"/>
+    </row>
+    <row r="159" spans="2:6">
+      <c r="B159" s="4" t="s">
+        <v>882</v>
+      </c>
+      <c r="C159" s="5"/>
+      <c r="D159" s="5"/>
+      <c r="E159" s="5"/>
+      <c r="F159" s="6"/>
+    </row>
+    <row r="160" spans="2:6">
+      <c r="B160" s="4" t="s">
+        <v>883</v>
+      </c>
+      <c r="C160" s="5"/>
+      <c r="D160" s="5"/>
+      <c r="E160" s="5"/>
+      <c r="F160" s="6"/>
+    </row>
+    <row r="161" spans="2:6">
+      <c r="B161" s="4" t="s">
+        <v>884</v>
+      </c>
+      <c r="C161" s="5"/>
+      <c r="D161" s="5"/>
+      <c r="E161" s="5"/>
+      <c r="F161" s="6"/>
+    </row>
+    <row r="162" spans="2:6">
+      <c r="B162" s="4" t="s">
+        <v>885</v>
+      </c>
+      <c r="C162" s="5"/>
+      <c r="D162" s="5"/>
+      <c r="E162" s="5"/>
+      <c r="F162" s="6"/>
+    </row>
+    <row r="163" spans="2:6">
+      <c r="B163" s="4" t="s">
+        <v>886</v>
+      </c>
+      <c r="C163" s="5"/>
+      <c r="D163" s="5"/>
+      <c r="E163" s="5"/>
+      <c r="F163" s="6"/>
+    </row>
+    <row r="164" spans="2:6">
+      <c r="B164" s="4" t="s">
+        <v>887</v>
+      </c>
+      <c r="C164" s="5"/>
+      <c r="D164" s="5"/>
+      <c r="E164" s="5"/>
+      <c r="F164" s="6"/>
+    </row>
+    <row r="165" spans="2:6">
+      <c r="B165" s="4" t="s">
+        <v>888</v>
+      </c>
+      <c r="C165" s="5"/>
+      <c r="D165" s="5"/>
+      <c r="E165" s="5"/>
+      <c r="F165" s="6"/>
+    </row>
+    <row r="166" spans="2:6">
+      <c r="B166" s="4" t="s">
+        <v>889</v>
+      </c>
+      <c r="C166" s="5"/>
+      <c r="D166" s="5"/>
+      <c r="E166" s="5"/>
+      <c r="F166" s="6"/>
+    </row>
+    <row r="167" spans="2:6">
+      <c r="B167" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="C167" s="5"/>
+      <c r="D167" s="5"/>
+      <c r="E167" s="5"/>
+      <c r="F167" s="6"/>
+    </row>
+    <row r="168" spans="2:6">
+      <c r="B168" s="4" t="s">
+        <v>891</v>
+      </c>
+      <c r="C168" s="5"/>
+      <c r="D168" s="5"/>
+      <c r="E168" s="5"/>
+      <c r="F168" s="6"/>
+    </row>
+    <row r="169" spans="2:6">
+      <c r="B169" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="C169" s="5"/>
+      <c r="D169" s="5"/>
+      <c r="E169" s="5"/>
+      <c r="F169" s="6"/>
+    </row>
+    <row r="170" spans="2:6">
+      <c r="B170" s="4" t="s">
+        <v>893</v>
+      </c>
+      <c r="C170" s="5"/>
+      <c r="D170" s="5"/>
+      <c r="E170" s="5"/>
+      <c r="F170" s="6"/>
+    </row>
+    <row r="171" spans="2:6">
+      <c r="B171" s="4" t="s">
+        <v>861</v>
+      </c>
+      <c r="C171" s="5"/>
+      <c r="D171" s="5"/>
+      <c r="E171" s="5"/>
+      <c r="F171" s="6"/>
+    </row>
+    <row r="172" spans="2:6">
+      <c r="B172" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="C172" s="5"/>
+      <c r="D172" s="5"/>
+      <c r="E172" s="5"/>
+      <c r="F172" s="6"/>
+    </row>
+    <row r="173" spans="2:6">
+      <c r="B173" s="4" t="s">
+        <v>895</v>
+      </c>
+      <c r="C173" s="5"/>
+      <c r="D173" s="5"/>
+      <c r="E173" s="5"/>
+      <c r="F173" s="6"/>
+    </row>
+    <row r="174" spans="2:6">
+      <c r="B174" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="C174" s="5"/>
+      <c r="D174" s="5"/>
+      <c r="E174" s="5"/>
+      <c r="F174" s="6"/>
+    </row>
+    <row r="175" spans="2:6">
+      <c r="B175" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C175" s="5"/>
+      <c r="D175" s="5"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="6"/>
+    </row>
+    <row r="176" spans="2:6">
+      <c r="B176" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C176" s="5"/>
+      <c r="D176" s="5"/>
+      <c r="E176" s="5"/>
+      <c r="F176" s="6"/>
+    </row>
+    <row r="177" spans="2:6">
+      <c r="B177" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C177" s="5"/>
+      <c r="D177" s="5"/>
+      <c r="E177" s="5"/>
+      <c r="F177" s="6"/>
+    </row>
+    <row r="178" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B178" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C178" s="8"/>
+      <c r="D178" s="8"/>
+      <c r="E178" s="8"/>
+      <c r="F178" s="9"/>
+    </row>
+    <row r="179" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="180" spans="2:6">
+      <c r="B180" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
+      <c r="E180" s="2"/>
+      <c r="F180" s="3"/>
+    </row>
+    <row r="181" spans="2:6">
+      <c r="B181" s="4"/>
+      <c r="C181" s="5"/>
+      <c r="D181" s="5"/>
+      <c r="E181" s="5"/>
+      <c r="F181" s="6"/>
+    </row>
+    <row r="182" spans="2:6">
+      <c r="B182" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C182" s="5"/>
+      <c r="D182" s="5"/>
+      <c r="E182" s="5"/>
+      <c r="F182" s="6"/>
+    </row>
+    <row r="183" spans="2:6">
+      <c r="B183" s="4" t="s">
+        <v>896</v>
+      </c>
+      <c r="C183" s="5"/>
+      <c r="D183" s="5"/>
+      <c r="E183" s="5"/>
+      <c r="F183" s="6"/>
+    </row>
+    <row r="184" spans="2:6">
+      <c r="B184" s="4" t="s">
+        <v>897</v>
+      </c>
+      <c r="C184" s="5"/>
+      <c r="D184" s="5"/>
+      <c r="E184" s="5"/>
+      <c r="F184" s="6"/>
+    </row>
+    <row r="185" spans="2:6">
+      <c r="B185" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="C185" s="5"/>
+      <c r="D185" s="5"/>
+      <c r="E185" s="5"/>
+      <c r="F185" s="6"/>
+    </row>
+    <row r="186" spans="2:6">
+      <c r="B186" s="4" t="s">
+        <v>899</v>
+      </c>
+      <c r="C186" s="5"/>
+      <c r="D186" s="5"/>
+      <c r="E186" s="5"/>
+      <c r="F186" s="6"/>
+    </row>
+    <row r="187" spans="2:6">
+      <c r="B187" s="4"/>
+      <c r="C187" s="5"/>
+      <c r="D187" s="5"/>
+      <c r="E187" s="5"/>
+      <c r="F187" s="6"/>
+    </row>
+    <row r="188" spans="2:6">
+      <c r="B188" s="4"/>
+      <c r="C188" s="5"/>
+      <c r="D188" s="5"/>
+      <c r="E188" s="5"/>
+      <c r="F188" s="6"/>
+    </row>
+    <row r="189" spans="2:6">
+      <c r="B189" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C189" s="5"/>
+      <c r="D189" s="5"/>
+      <c r="E189" s="5"/>
+      <c r="F189" s="6"/>
+    </row>
+    <row r="190" spans="2:6">
+      <c r="B190" s="4" t="s">
+        <v>900</v>
+      </c>
+      <c r="C190" s="5"/>
+      <c r="D190" s="5"/>
+      <c r="E190" s="5"/>
+      <c r="F190" s="6"/>
+    </row>
+    <row r="191" spans="2:6">
+      <c r="B191" s="4" t="s">
+        <v>901</v>
+      </c>
+      <c r="C191" s="5"/>
+      <c r="D191" s="5"/>
+      <c r="E191" s="5"/>
+      <c r="F191" s="6"/>
+    </row>
+    <row r="192" spans="2:6">
+      <c r="B192" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="5"/>
+      <c r="F192" s="6"/>
+    </row>
+    <row r="193" spans="2:6">
+      <c r="B193" s="4" t="s">
+        <v>903</v>
+      </c>
+      <c r="C193" s="5"/>
+      <c r="D193" s="5"/>
+      <c r="E193" s="5"/>
+      <c r="F193" s="6"/>
+    </row>
+    <row r="194" spans="2:6">
+      <c r="B194" s="4"/>
+      <c r="C194" s="5"/>
+      <c r="D194" s="5"/>
+      <c r="E194" s="5"/>
+      <c r="F194" s="6"/>
+    </row>
+    <row r="195" spans="2:6">
+      <c r="B195" s="4"/>
+      <c r="C195" s="5"/>
+      <c r="D195" s="5"/>
+      <c r="E195" s="5"/>
+      <c r="F195" s="6"/>
+    </row>
+    <row r="196" spans="2:6">
+      <c r="B196" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C196" s="5"/>
+      <c r="D196" s="5"/>
+      <c r="E196" s="5"/>
+      <c r="F196" s="6"/>
+    </row>
+    <row r="197" spans="2:6">
+      <c r="B197" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D197" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E197" s="5"/>
+      <c r="F197" s="6"/>
+    </row>
+    <row r="198" spans="2:6">
+      <c r="B198" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D198" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E198" s="5"/>
+      <c r="F198" s="6"/>
+    </row>
+    <row r="199" spans="2:6">
+      <c r="B199" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C199" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D199" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E199" s="5"/>
+      <c r="F199" s="6"/>
+    </row>
+    <row r="200" spans="2:6">
+      <c r="B200" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C200" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D200" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E200" s="5"/>
+      <c r="F200" s="6"/>
+    </row>
+    <row r="201" spans="2:6">
+      <c r="B201" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C201" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D201" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E201" s="5"/>
+      <c r="F201" s="6"/>
+    </row>
+    <row r="202" spans="2:6">
+      <c r="B202" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E202" s="5"/>
+      <c r="F202" s="6"/>
+    </row>
+    <row r="203" spans="2:6">
+      <c r="B203" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C203" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D203" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="E203" s="5"/>
+      <c r="F203" s="6"/>
+    </row>
+    <row r="204" spans="2:6">
+      <c r="B204" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C204" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D204" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E204" s="5"/>
+      <c r="F204" s="6"/>
+    </row>
+    <row r="205" spans="2:6">
+      <c r="B205" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E205" s="5"/>
+      <c r="F205" s="6"/>
+    </row>
+    <row r="206" spans="2:6">
+      <c r="B206" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E206" s="5"/>
+      <c r="F206" s="6"/>
+    </row>
+    <row r="207" spans="2:6">
+      <c r="B207" s="4"/>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+      <c r="E207" s="5"/>
+      <c r="F207" s="6"/>
+    </row>
+    <row r="208" spans="2:6">
+      <c r="B208" s="4"/>
+      <c r="C208" s="5"/>
+      <c r="D208" s="5"/>
+      <c r="E208" s="5"/>
+      <c r="F208" s="6"/>
+    </row>
+    <row r="209" spans="2:6">
+      <c r="B209" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C209" s="5"/>
+      <c r="D209" s="5"/>
+      <c r="E209" s="5"/>
+      <c r="F209" s="6"/>
+    </row>
+    <row r="210" spans="2:6">
+      <c r="B210" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C210" s="5"/>
+      <c r="D210" s="5"/>
+      <c r="E210" s="5"/>
+      <c r="F210" s="6"/>
+    </row>
+    <row r="211" spans="2:6">
+      <c r="B211" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C211" s="5"/>
+      <c r="D211" s="5"/>
+      <c r="E211" s="5"/>
+      <c r="F211" s="6"/>
+    </row>
+    <row r="212" spans="2:6">
+      <c r="B212" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C212" s="5"/>
+      <c r="D212" s="5"/>
+      <c r="E212" s="5"/>
+      <c r="F212" s="6"/>
+    </row>
+    <row r="213" spans="2:6">
+      <c r="B213" s="4" t="s">
+        <v>904</v>
+      </c>
+      <c r="C213" s="5"/>
+      <c r="D213" s="5"/>
+      <c r="E213" s="5"/>
+      <c r="F213" s="6"/>
+    </row>
+    <row r="214" spans="2:6">
+      <c r="B214" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="C214" s="5"/>
+      <c r="D214" s="5"/>
+      <c r="E214" s="5"/>
+      <c r="F214" s="6"/>
+    </row>
+    <row r="215" spans="2:6">
+      <c r="B215" s="4" t="s">
+        <v>905</v>
+      </c>
+      <c r="C215" s="5"/>
+      <c r="D215" s="5"/>
+      <c r="E215" s="5"/>
+      <c r="F215" s="6"/>
+    </row>
+    <row r="216" spans="2:6">
+      <c r="B216" s="4" t="s">
+        <v>906</v>
+      </c>
+      <c r="C216" s="5"/>
+      <c r="D216" s="5"/>
+      <c r="E216" s="5"/>
+      <c r="F216" s="6"/>
+    </row>
+    <row r="217" spans="2:6">
+      <c r="B217" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="C217" s="5"/>
+      <c r="D217" s="5"/>
+      <c r="E217" s="5"/>
+      <c r="F217" s="6"/>
+    </row>
+    <row r="218" spans="2:6">
+      <c r="B218" s="4" t="s">
+        <v>907</v>
+      </c>
+      <c r="C218" s="5"/>
+      <c r="D218" s="5"/>
+      <c r="E218" s="5"/>
+      <c r="F218" s="6"/>
+    </row>
+    <row r="219" spans="2:6">
+      <c r="B219" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C219" s="5"/>
+      <c r="D219" s="5"/>
+      <c r="E219" s="5"/>
+      <c r="F219" s="6"/>
+    </row>
+    <row r="220" spans="2:6">
+      <c r="B220" s="4" t="s">
+        <v>908</v>
+      </c>
+      <c r="C220" s="5"/>
+      <c r="D220" s="5"/>
+      <c r="E220" s="5"/>
+      <c r="F220" s="6"/>
+    </row>
+    <row r="221" spans="2:6">
+      <c r="B221" s="4" t="s">
+        <v>909</v>
+      </c>
+      <c r="C221" s="5"/>
+      <c r="D221" s="5"/>
+      <c r="E221" s="5"/>
+      <c r="F221" s="6"/>
+    </row>
+    <row r="222" spans="2:6">
+      <c r="B222" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="C222" s="5"/>
+      <c r="D222" s="5"/>
+      <c r="E222" s="5"/>
+      <c r="F222" s="6"/>
+    </row>
+    <row r="223" spans="2:6">
+      <c r="B223" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5"/>
+      <c r="E223" s="5"/>
+      <c r="F223" s="6"/>
+    </row>
+    <row r="224" spans="2:6">
+      <c r="B224" s="4" t="s">
+        <v>911</v>
+      </c>
+      <c r="C224" s="5"/>
+      <c r="D224" s="5"/>
+      <c r="E224" s="5"/>
+      <c r="F224" s="6"/>
+    </row>
+    <row r="225" spans="2:6">
+      <c r="B225" s="4" t="s">
+        <v>912</v>
+      </c>
+      <c r="C225" s="5"/>
+      <c r="D225" s="5"/>
+      <c r="E225" s="5"/>
+      <c r="F225" s="6"/>
+    </row>
+    <row r="226" spans="2:6">
+      <c r="B226" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="C226" s="5"/>
+      <c r="D226" s="5"/>
+      <c r="E226" s="5"/>
+      <c r="F226" s="6"/>
+    </row>
+    <row r="227" spans="2:6">
+      <c r="B227" s="4" t="s">
+        <v>914</v>
+      </c>
+      <c r="C227" s="5"/>
+      <c r="D227" s="5"/>
+      <c r="E227" s="5"/>
+      <c r="F227" s="6"/>
+    </row>
+    <row r="228" spans="2:6">
+      <c r="B228" s="4" t="s">
+        <v>915</v>
+      </c>
+      <c r="C228" s="5"/>
+      <c r="D228" s="5"/>
+      <c r="E228" s="5"/>
+      <c r="F228" s="6"/>
+    </row>
+    <row r="229" spans="2:6">
+      <c r="B229" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="C229" s="5"/>
+      <c r="D229" s="5"/>
+      <c r="E229" s="5"/>
+      <c r="F229" s="6"/>
+    </row>
+    <row r="230" spans="2:6">
+      <c r="B230" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="C230" s="5"/>
+      <c r="D230" s="5"/>
+      <c r="E230" s="5"/>
+      <c r="F230" s="6"/>
+    </row>
+    <row r="231" spans="2:6">
+      <c r="B231" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="C231" s="5"/>
+      <c r="D231" s="5"/>
+      <c r="E231" s="5"/>
+      <c r="F231" s="6"/>
+    </row>
+    <row r="232" spans="2:6">
+      <c r="B232" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C232" s="5"/>
+      <c r="D232" s="5"/>
+      <c r="E232" s="5"/>
+      <c r="F232" s="6"/>
+    </row>
+    <row r="233" spans="2:6">
+      <c r="B233" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C233" s="5"/>
+      <c r="D233" s="5"/>
+      <c r="E233" s="5"/>
+      <c r="F233" s="6"/>
+    </row>
+    <row r="234" spans="2:6">
+      <c r="B234" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C234" s="5"/>
+      <c r="D234" s="5"/>
+      <c r="E234" s="5"/>
+      <c r="F234" s="6"/>
+    </row>
+    <row r="235" spans="2:6">
+      <c r="B235" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="C235" s="5"/>
+      <c r="D235" s="5"/>
+      <c r="E235" s="5"/>
+      <c r="F235" s="6"/>
+    </row>
+    <row r="236" spans="2:6">
+      <c r="B236" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="C236" s="5"/>
+      <c r="D236" s="5"/>
+      <c r="E236" s="5"/>
+      <c r="F236" s="6"/>
+    </row>
+    <row r="237" spans="2:6">
+      <c r="B237" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C237" s="5"/>
+      <c r="D237" s="5"/>
+      <c r="E237" s="5"/>
+      <c r="F237" s="6"/>
+    </row>
+    <row r="238" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B238" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C238" s="8"/>
+      <c r="D238" s="8"/>
+      <c r="E238" s="8"/>
+      <c r="F238" s="9"/>
+    </row>
+    <row r="239" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="240" spans="2:6">
+      <c r="B240" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="C240" s="2"/>
+      <c r="D240" s="2"/>
+      <c r="E240" s="2"/>
+      <c r="F240" s="3"/>
+    </row>
+    <row r="241" spans="2:6">
+      <c r="B241" s="4"/>
+      <c r="C241" s="5"/>
+      <c r="D241" s="5"/>
+      <c r="E241" s="5"/>
+      <c r="F241" s="6"/>
+    </row>
+    <row r="242" spans="2:6">
+      <c r="B242" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C242" s="5"/>
+      <c r="D242" s="5"/>
+      <c r="E242" s="5"/>
+      <c r="F242" s="6"/>
+    </row>
+    <row r="243" spans="2:6">
+      <c r="B243" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="C243" s="5"/>
+      <c r="D243" s="5"/>
+      <c r="E243" s="5"/>
+      <c r="F243" s="6"/>
+    </row>
+    <row r="244" spans="2:6">
+      <c r="B244" s="4" t="s">
+        <v>921</v>
+      </c>
+      <c r="C244" s="5"/>
+      <c r="D244" s="5"/>
+      <c r="E244" s="5"/>
+      <c r="F244" s="6"/>
+    </row>
+    <row r="245" spans="2:6">
+      <c r="B245" s="4" t="s">
+        <v>922</v>
+      </c>
+      <c r="C245" s="5"/>
+      <c r="D245" s="5"/>
+      <c r="E245" s="5"/>
+      <c r="F245" s="6"/>
+    </row>
+    <row r="246" spans="2:6">
+      <c r="B246" s="4" t="s">
+        <v>923</v>
+      </c>
+      <c r="C246" s="5"/>
+      <c r="D246" s="5"/>
+      <c r="E246" s="5"/>
+      <c r="F246" s="6"/>
+    </row>
+    <row r="247" spans="2:6">
+      <c r="B247" s="4"/>
+      <c r="C247" s="5"/>
+      <c r="D247" s="5"/>
+      <c r="E247" s="5"/>
+      <c r="F247" s="6"/>
+    </row>
+    <row r="248" spans="2:6">
+      <c r="B248" s="4"/>
+      <c r="C248" s="5"/>
+      <c r="D248" s="5"/>
+      <c r="E248" s="5"/>
+      <c r="F248" s="6"/>
+    </row>
+    <row r="249" spans="2:6">
+      <c r="B249" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C249" s="5"/>
+      <c r="D249" s="5"/>
+      <c r="E249" s="5"/>
+      <c r="F249" s="6"/>
+    </row>
+    <row r="250" spans="2:6">
+      <c r="B250" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="C250" s="5"/>
+      <c r="D250" s="5"/>
+      <c r="E250" s="5"/>
+      <c r="F250" s="6"/>
+    </row>
+    <row r="251" spans="2:6">
+      <c r="B251" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="C251" s="5"/>
+      <c r="D251" s="5"/>
+      <c r="E251" s="5"/>
+      <c r="F251" s="6"/>
+    </row>
+    <row r="252" spans="2:6">
+      <c r="B252" s="4" t="s">
+        <v>926</v>
+      </c>
+      <c r="C252" s="5"/>
+      <c r="D252" s="5"/>
+      <c r="E252" s="5"/>
+      <c r="F252" s="6"/>
+    </row>
+    <row r="253" spans="2:6">
+      <c r="B253" s="4" t="s">
+        <v>927</v>
+      </c>
+      <c r="C253" s="5"/>
+      <c r="D253" s="5"/>
+      <c r="E253" s="5"/>
+      <c r="F253" s="6"/>
+    </row>
+    <row r="254" spans="2:6">
+      <c r="B254" s="4"/>
+      <c r="C254" s="5"/>
+      <c r="D254" s="5"/>
+      <c r="E254" s="5"/>
+      <c r="F254" s="6"/>
+    </row>
+    <row r="255" spans="2:6">
+      <c r="B255" s="4"/>
+      <c r="C255" s="5"/>
+      <c r="D255" s="5"/>
+      <c r="E255" s="5"/>
+      <c r="F255" s="6"/>
+    </row>
+    <row r="256" spans="2:6">
+      <c r="B256" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C256" s="5"/>
+      <c r="D256" s="5"/>
+      <c r="E256" s="5"/>
+      <c r="F256" s="6"/>
+    </row>
+    <row r="257" spans="2:6">
+      <c r="B257" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="C257" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E257" s="5"/>
+      <c r="F257" s="6"/>
+    </row>
+    <row r="258" spans="2:6">
+      <c r="B258" s="4" t="s">
+        <v>929</v>
+      </c>
+      <c r="C258" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D258" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E258" s="5"/>
+      <c r="F258" s="6"/>
+    </row>
+    <row r="259" spans="2:6">
+      <c r="B259" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="C259" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D259" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E259" s="5"/>
+      <c r="F259" s="6"/>
+    </row>
+    <row r="260" spans="2:6">
+      <c r="B260" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C260" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D260" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E260" s="5"/>
+      <c r="F260" s="6"/>
+    </row>
+    <row r="261" spans="2:6">
+      <c r="B261" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="C261" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D261" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E261" s="5"/>
+      <c r="F261" s="6"/>
+    </row>
+    <row r="262" spans="2:6">
+      <c r="B262" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C262" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D262" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E262" s="5"/>
+      <c r="F262" s="6"/>
+    </row>
+    <row r="263" spans="2:6">
+      <c r="B263" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="C263" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D263" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E263" s="5"/>
+      <c r="F263" s="6"/>
+    </row>
+    <row r="264" spans="2:6">
+      <c r="B264" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C264" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D264" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="E264" s="5"/>
+      <c r="F264" s="6"/>
+    </row>
+    <row r="265" spans="2:6">
+      <c r="B265" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C265" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D265" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E265" s="5"/>
+      <c r="F265" s="6"/>
+    </row>
+    <row r="266" spans="2:6">
+      <c r="B266" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C266" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D266" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E266" s="5"/>
+      <c r="F266" s="6"/>
+    </row>
+    <row r="267" spans="2:6">
+      <c r="B267" s="4"/>
+      <c r="C267" s="5"/>
+      <c r="D267" s="5"/>
+      <c r="E267" s="5"/>
+      <c r="F267" s="6"/>
+    </row>
+    <row r="268" spans="2:6">
+      <c r="B268" s="4"/>
+      <c r="C268" s="5"/>
+      <c r="D268" s="5"/>
+      <c r="E268" s="5"/>
+      <c r="F268" s="6"/>
+    </row>
+    <row r="269" spans="2:6">
+      <c r="B269" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C269" s="5"/>
+      <c r="D269" s="5"/>
+      <c r="E269" s="5"/>
+      <c r="F269" s="6"/>
+    </row>
+    <row r="270" spans="2:6">
+      <c r="B270" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C270" s="5"/>
+      <c r="D270" s="5"/>
+      <c r="E270" s="5"/>
+      <c r="F270" s="6"/>
+    </row>
+    <row r="271" spans="2:6">
+      <c r="B271" s="4" t="s">
+        <v>931</v>
+      </c>
+      <c r="C271" s="5"/>
+      <c r="D271" s="5"/>
+      <c r="E271" s="5"/>
+      <c r="F271" s="6"/>
+    </row>
+    <row r="272" spans="2:6">
+      <c r="B272" s="4" t="s">
+        <v>866</v>
+      </c>
+      <c r="C272" s="5"/>
+      <c r="D272" s="5"/>
+      <c r="E272" s="5"/>
+      <c r="F272" s="6"/>
+    </row>
+    <row r="273" spans="2:6">
+      <c r="B273" s="4" t="s">
+        <v>932</v>
+      </c>
+      <c r="C273" s="5"/>
+      <c r="D273" s="5"/>
+      <c r="E273" s="5"/>
+      <c r="F273" s="6"/>
+    </row>
+    <row r="274" spans="2:6">
+      <c r="B274" s="4" t="s">
+        <v>933</v>
+      </c>
+      <c r="C274" s="5"/>
+      <c r="D274" s="5"/>
+      <c r="E274" s="5"/>
+      <c r="F274" s="6"/>
+    </row>
+    <row r="275" spans="2:6">
+      <c r="B275" s="4" t="s">
+        <v>934</v>
+      </c>
+      <c r="C275" s="5"/>
+      <c r="D275" s="5"/>
+      <c r="E275" s="5"/>
+      <c r="F275" s="6"/>
+    </row>
+    <row r="276" spans="2:6">
+      <c r="B276" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="C276" s="5"/>
+      <c r="D276" s="5"/>
+      <c r="E276" s="5"/>
+      <c r="F276" s="6"/>
+    </row>
+    <row r="277" spans="2:6">
+      <c r="B277" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="C277" s="5"/>
+      <c r="D277" s="5"/>
+      <c r="E277" s="5"/>
+      <c r="F277" s="6"/>
+    </row>
+    <row r="278" spans="2:6">
+      <c r="B278" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="C278" s="5"/>
+      <c r="D278" s="5"/>
+      <c r="E278" s="5"/>
+      <c r="F278" s="6"/>
+    </row>
+    <row r="279" spans="2:6">
+      <c r="B279" s="4" t="s">
+        <v>938</v>
+      </c>
+      <c r="C279" s="5"/>
+      <c r="D279" s="5"/>
+      <c r="E279" s="5"/>
+      <c r="F279" s="6"/>
+    </row>
+    <row r="280" spans="2:6">
+      <c r="B280" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="C280" s="5"/>
+      <c r="D280" s="5"/>
+      <c r="E280" s="5"/>
+      <c r="F280" s="6"/>
+    </row>
+    <row r="281" spans="2:6">
+      <c r="B281" s="4" t="s">
+        <v>940</v>
+      </c>
+      <c r="C281" s="5"/>
+      <c r="D281" s="5"/>
+      <c r="E281" s="5"/>
+      <c r="F281" s="6"/>
+    </row>
+    <row r="282" spans="2:6">
+      <c r="B282" s="4" t="s">
+        <v>941</v>
+      </c>
+      <c r="C282" s="5"/>
+      <c r="D282" s="5"/>
+      <c r="E282" s="5"/>
+      <c r="F282" s="6"/>
+    </row>
+    <row r="283" spans="2:6">
+      <c r="B283" s="4" t="s">
+        <v>942</v>
+      </c>
+      <c r="C283" s="5"/>
+      <c r="D283" s="5"/>
+      <c r="E283" s="5"/>
+      <c r="F283" s="6"/>
+    </row>
+    <row r="284" spans="2:6">
+      <c r="B284" s="4" t="s">
+        <v>943</v>
+      </c>
+      <c r="C284" s="5"/>
+      <c r="D284" s="5"/>
+      <c r="E284" s="5"/>
+      <c r="F284" s="6"/>
+    </row>
+    <row r="285" spans="2:6">
+      <c r="B285" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="C285" s="5"/>
+      <c r="D285" s="5"/>
+      <c r="E285" s="5"/>
+      <c r="F285" s="6"/>
+    </row>
+    <row r="286" spans="2:6">
+      <c r="B286" s="4" t="s">
+        <v>945</v>
+      </c>
+      <c r="C286" s="5"/>
+      <c r="D286" s="5"/>
+      <c r="E286" s="5"/>
+      <c r="F286" s="6"/>
+    </row>
+    <row r="287" spans="2:6">
+      <c r="B287" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="C287" s="5"/>
+      <c r="D287" s="5"/>
+      <c r="E287" s="5"/>
+      <c r="F287" s="6"/>
+    </row>
+    <row r="288" spans="2:6">
+      <c r="B288" s="4" t="s">
+        <v>947</v>
+      </c>
+      <c r="C288" s="5"/>
+      <c r="D288" s="5"/>
+      <c r="E288" s="5"/>
+      <c r="F288" s="6"/>
+    </row>
+    <row r="289" spans="2:6">
+      <c r="B289" s="4" t="s">
+        <v>948</v>
+      </c>
+      <c r="C289" s="5"/>
+      <c r="D289" s="5"/>
+      <c r="E289" s="5"/>
+      <c r="F289" s="6"/>
+    </row>
+    <row r="290" spans="2:6">
+      <c r="B290" s="4" t="s">
+        <v>949</v>
+      </c>
+      <c r="C290" s="5"/>
+      <c r="D290" s="5"/>
+      <c r="E290" s="5"/>
+      <c r="F290" s="6"/>
+    </row>
+    <row r="291" spans="2:6">
+      <c r="B291" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="C291" s="5"/>
+      <c r="D291" s="5"/>
+      <c r="E291" s="5"/>
+      <c r="F291" s="6"/>
+    </row>
+    <row r="292" spans="2:6">
+      <c r="B292" s="4" t="s">
+        <v>951</v>
+      </c>
+      <c r="C292" s="5"/>
+      <c r="D292" s="5"/>
+      <c r="E292" s="5"/>
+      <c r="F292" s="6"/>
+    </row>
+    <row r="293" spans="2:6">
+      <c r="B293" s="4" t="s">
+        <v>952</v>
+      </c>
+      <c r="C293" s="5"/>
+      <c r="D293" s="5"/>
+      <c r="E293" s="5"/>
+      <c r="F293" s="6"/>
+    </row>
+    <row r="294" spans="2:6">
+      <c r="B294" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C294" s="5"/>
+      <c r="D294" s="5"/>
+      <c r="E294" s="5"/>
+      <c r="F294" s="6"/>
+    </row>
+    <row r="295" spans="2:6">
+      <c r="B295" s="4" t="s">
+        <v>953</v>
+      </c>
+      <c r="C295" s="5"/>
+      <c r="D295" s="5"/>
+      <c r="E295" s="5"/>
+      <c r="F295" s="6"/>
+    </row>
+    <row r="296" spans="2:6">
+      <c r="B296" s="4" t="s">
+        <v>954</v>
+      </c>
+      <c r="C296" s="5"/>
+      <c r="D296" s="5"/>
+      <c r="E296" s="5"/>
+      <c r="F296" s="6"/>
+    </row>
+    <row r="297" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B297" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C297" s="8"/>
+      <c r="D297" s="8"/>
+      <c r="E297" s="8"/>
+      <c r="F297" s="9"/>
+    </row>
+    <row r="298" spans="2:6" ht="15.75" thickBot="1"/>
+    <row r="299" spans="2:6">
+      <c r="B299" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C299" s="2"/>
+      <c r="D299" s="2"/>
+      <c r="E299" s="2"/>
+      <c r="F299" s="3"/>
+    </row>
+    <row r="300" spans="2:6">
+      <c r="B300" s="4"/>
+      <c r="C300" s="5"/>
+      <c r="D300" s="5"/>
+      <c r="E300" s="5"/>
+      <c r="F300" s="6"/>
+    </row>
+    <row r="301" spans="2:6">
+      <c r="B301" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C301" s="5"/>
+      <c r="D301" s="5"/>
+      <c r="E301" s="5"/>
+      <c r="F301" s="6"/>
+    </row>
+    <row r="302" spans="2:6">
+      <c r="B302" s="4" t="s">
+        <v>956</v>
+      </c>
+      <c r="C302" s="5"/>
+      <c r="D302" s="5"/>
+      <c r="E302" s="5"/>
+      <c r="F302" s="6"/>
+    </row>
+    <row r="303" spans="2:6">
+      <c r="B303" s="4" t="s">
+        <v>957</v>
+      </c>
+      <c r="C303" s="5"/>
+      <c r="D303" s="5"/>
+      <c r="E303" s="5"/>
+      <c r="F303" s="6"/>
+    </row>
+    <row r="304" spans="2:6">
+      <c r="B304" s="4" t="s">
+        <v>958</v>
+      </c>
+      <c r="C304" s="5"/>
+      <c r="D304" s="5"/>
+      <c r="E304" s="5"/>
+      <c r="F304" s="6"/>
+    </row>
+    <row r="305" spans="2:6">
+      <c r="B305" s="4" t="s">
+        <v>959</v>
+      </c>
+      <c r="C305" s="5"/>
+      <c r="D305" s="5"/>
+      <c r="E305" s="5"/>
+      <c r="F305" s="6"/>
+    </row>
+    <row r="306" spans="2:6">
+      <c r="B306" s="4"/>
+      <c r="C306" s="5"/>
+      <c r="D306" s="5"/>
+      <c r="E306" s="5"/>
+      <c r="F306" s="6"/>
+    </row>
+    <row r="307" spans="2:6">
+      <c r="B307" s="4"/>
+      <c r="C307" s="5"/>
+      <c r="D307" s="5"/>
+      <c r="E307" s="5"/>
+      <c r="F307" s="6"/>
+    </row>
+    <row r="308" spans="2:6">
+      <c r="B308" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C308" s="5"/>
+      <c r="D308" s="5"/>
+      <c r="E308" s="5"/>
+      <c r="F308" s="6"/>
+    </row>
+    <row r="309" spans="2:6">
+      <c r="B309" s="4" t="s">
+        <v>960</v>
+      </c>
+      <c r="C309" s="5"/>
+      <c r="D309" s="5"/>
+      <c r="E309" s="5"/>
+      <c r="F309" s="6"/>
+    </row>
+    <row r="310" spans="2:6">
+      <c r="B310" s="4" t="s">
+        <v>961</v>
+      </c>
+      <c r="C310" s="5"/>
+      <c r="D310" s="5"/>
+      <c r="E310" s="5"/>
+      <c r="F310" s="6"/>
+    </row>
+    <row r="311" spans="2:6">
+      <c r="B311" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="C311" s="5"/>
+      <c r="D311" s="5"/>
+      <c r="E311" s="5"/>
+      <c r="F311" s="6"/>
+    </row>
+    <row r="312" spans="2:6">
+      <c r="B312" s="4" t="s">
+        <v>963</v>
+      </c>
+      <c r="C312" s="5"/>
+      <c r="D312" s="5"/>
+      <c r="E312" s="5"/>
+      <c r="F312" s="6"/>
+    </row>
+    <row r="313" spans="2:6">
+      <c r="B313" s="4"/>
+      <c r="C313" s="5"/>
+      <c r="D313" s="5"/>
+      <c r="E313" s="5"/>
+      <c r="F313" s="6"/>
+    </row>
+    <row r="314" spans="2:6">
+      <c r="B314" s="4"/>
+      <c r="C314" s="5"/>
+      <c r="D314" s="5"/>
+      <c r="E314" s="5"/>
+      <c r="F314" s="6"/>
+    </row>
+    <row r="315" spans="2:6">
+      <c r="B315" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C315" s="5"/>
+      <c r="D315" s="5"/>
+      <c r="E315" s="5"/>
+      <c r="F315" s="6"/>
+    </row>
+    <row r="316" spans="2:6">
+      <c r="B316" s="4" t="s">
+        <v>964</v>
+      </c>
+      <c r="C316" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D316" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E316" s="5"/>
+      <c r="F316" s="6"/>
+    </row>
+    <row r="317" spans="2:6">
+      <c r="B317" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C317" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D317" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E317" s="5"/>
+      <c r="F317" s="6"/>
+    </row>
+    <row r="318" spans="2:6">
+      <c r="B318" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C318" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D318" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E318" s="5"/>
+      <c r="F318" s="6"/>
+    </row>
+    <row r="319" spans="2:6">
+      <c r="B319" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C319" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D319" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E319" s="5"/>
+      <c r="F319" s="6"/>
+    </row>
+    <row r="320" spans="2:6">
+      <c r="B320" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C320" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D320" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E320" s="5"/>
+      <c r="F320" s="6"/>
+    </row>
+    <row r="321" spans="2:6">
+      <c r="B321" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C321" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D321" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E321" s="5"/>
+      <c r="F321" s="6"/>
+    </row>
+    <row r="322" spans="2:6">
+      <c r="B322" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C322" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D322" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="E322" s="5"/>
+      <c r="F322" s="6"/>
+    </row>
+    <row r="323" spans="2:6">
+      <c r="B323" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C323" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D323" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E323" s="5"/>
+      <c r="F323" s="6"/>
+    </row>
+    <row r="324" spans="2:6">
+      <c r="B324" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C324" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D324" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E324" s="5"/>
+      <c r="F324" s="6"/>
+    </row>
+    <row r="325" spans="2:6">
+      <c r="B325" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C325" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D325" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="E325" s="5"/>
+      <c r="F325" s="6"/>
+    </row>
+    <row r="326" spans="2:6">
+      <c r="B326" s="4"/>
+      <c r="C326" s="5"/>
+      <c r="D326" s="5"/>
+      <c r="E326" s="5"/>
+      <c r="F326" s="6"/>
+    </row>
+    <row r="327" spans="2:6">
+      <c r="B327" s="4"/>
+      <c r="C327" s="5"/>
+      <c r="D327" s="5"/>
+      <c r="E327" s="5"/>
+      <c r="F327" s="6"/>
+    </row>
+    <row r="328" spans="2:6">
+      <c r="B328" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C328" s="5"/>
+      <c r="D328" s="5"/>
+      <c r="E328" s="5"/>
+      <c r="F328" s="6"/>
+    </row>
+    <row r="329" spans="2:6">
+      <c r="B329" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C329" s="5"/>
+      <c r="D329" s="5"/>
+      <c r="E329" s="5"/>
+      <c r="F329" s="6"/>
+    </row>
+    <row r="330" spans="2:6">
+      <c r="B330" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C330" s="5"/>
+      <c r="D330" s="5"/>
+      <c r="E330" s="5"/>
+      <c r="F330" s="6"/>
+    </row>
+    <row r="331" spans="2:6">
+      <c r="B331" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="C331" s="5"/>
+      <c r="D331" s="5"/>
+      <c r="E331" s="5"/>
+      <c r="F331" s="6"/>
+    </row>
+    <row r="332" spans="2:6">
+      <c r="B332" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C332" s="5"/>
+      <c r="D332" s="5"/>
+      <c r="E332" s="5"/>
+      <c r="F332" s="6"/>
+    </row>
+    <row r="333" spans="2:6">
+      <c r="B333" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="C333" s="5"/>
+      <c r="D333" s="5"/>
+      <c r="E333" s="5"/>
+      <c r="F333" s="6"/>
+    </row>
+    <row r="334" spans="2:6">
+      <c r="B334" s="4" t="s">
+        <v>966</v>
+      </c>
+      <c r="C334" s="5"/>
+      <c r="D334" s="5"/>
+      <c r="E334" s="5"/>
+      <c r="F334" s="6"/>
+    </row>
+    <row r="335" spans="2:6">
+      <c r="B335" s="4" t="s">
+        <v>967</v>
+      </c>
+      <c r="C335" s="5"/>
+      <c r="D335" s="5"/>
+      <c r="E335" s="5"/>
+      <c r="F335" s="6"/>
+    </row>
+    <row r="336" spans="2:6">
+      <c r="B336" s="4" t="s">
+        <v>968</v>
+      </c>
+      <c r="C336" s="5"/>
+      <c r="D336" s="5"/>
+      <c r="E336" s="5"/>
+      <c r="F336" s="6"/>
+    </row>
+    <row r="337" spans="2:6">
+      <c r="B337" s="4" t="s">
+        <v>969</v>
+      </c>
+      <c r="C337" s="5"/>
+      <c r="D337" s="5"/>
+      <c r="E337" s="5"/>
+      <c r="F337" s="6"/>
+    </row>
+    <row r="338" spans="2:6">
+      <c r="B338" s="4" t="s">
+        <v>970</v>
+      </c>
+      <c r="C338" s="5"/>
+      <c r="D338" s="5"/>
+      <c r="E338" s="5"/>
+      <c r="F338" s="6"/>
+    </row>
+    <row r="339" spans="2:6">
+      <c r="B339" s="4" t="s">
+        <v>971</v>
+      </c>
+      <c r="C339" s="5"/>
+      <c r="D339" s="5"/>
+      <c r="E339" s="5"/>
+      <c r="F339" s="6"/>
+    </row>
+    <row r="340" spans="2:6">
+      <c r="B340" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="C340" s="5"/>
+      <c r="D340" s="5"/>
+      <c r="E340" s="5"/>
+      <c r="F340" s="6"/>
+    </row>
+    <row r="341" spans="2:6">
+      <c r="B341" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="C341" s="5"/>
+      <c r="D341" s="5"/>
+      <c r="E341" s="5"/>
+      <c r="F341" s="6"/>
+    </row>
+    <row r="342" spans="2:6">
+      <c r="B342" s="4" t="s">
+        <v>974</v>
+      </c>
+      <c r="C342" s="5"/>
+      <c r="D342" s="5"/>
+      <c r="E342" s="5"/>
+      <c r="F342" s="6"/>
+    </row>
+    <row r="343" spans="2:6">
+      <c r="B343" s="4" t="s">
+        <v>975</v>
+      </c>
+      <c r="C343" s="5"/>
+      <c r="D343" s="5"/>
+      <c r="E343" s="5"/>
+      <c r="F343" s="6"/>
+    </row>
+    <row r="344" spans="2:6">
+      <c r="B344" s="4" t="s">
+        <v>976</v>
+      </c>
+      <c r="C344" s="5"/>
+      <c r="D344" s="5"/>
+      <c r="E344" s="5"/>
+      <c r="F344" s="6"/>
+    </row>
+    <row r="345" spans="2:6">
+      <c r="B345" s="4" t="s">
+        <v>977</v>
+      </c>
+      <c r="C345" s="5"/>
+      <c r="D345" s="5"/>
+      <c r="E345" s="5"/>
+      <c r="F345" s="6"/>
+    </row>
+    <row r="346" spans="2:6">
+      <c r="B346" s="4" t="s">
+        <v>978</v>
+      </c>
+      <c r="C346" s="5"/>
+      <c r="D346" s="5"/>
+      <c r="E346" s="5"/>
+      <c r="F346" s="6"/>
+    </row>
+    <row r="347" spans="2:6">
+      <c r="B347" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="C347" s="5"/>
+      <c r="D347" s="5"/>
+      <c r="E347" s="5"/>
+      <c r="F347" s="6"/>
+    </row>
+    <row r="348" spans="2:6">
+      <c r="B348" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="C348" s="5"/>
+      <c r="D348" s="5"/>
+      <c r="E348" s="5"/>
+      <c r="F348" s="6"/>
+    </row>
+    <row r="349" spans="2:6">
+      <c r="B349" s="4" t="s">
+        <v>981</v>
+      </c>
+      <c r="C349" s="5"/>
+      <c r="D349" s="5"/>
+      <c r="E349" s="5"/>
+      <c r="F349" s="6"/>
+    </row>
+    <row r="350" spans="2:6">
+      <c r="B350" s="4" t="s">
+        <v>982</v>
+      </c>
+      <c r="C350" s="5"/>
+      <c r="D350" s="5"/>
+      <c r="E350" s="5"/>
+      <c r="F350" s="6"/>
+    </row>
+    <row r="351" spans="2:6">
+      <c r="B351" s="4" t="s">
+        <v>983</v>
+      </c>
+      <c r="C351" s="5"/>
+      <c r="D351" s="5"/>
+      <c r="E351" s="5"/>
+      <c r="F351" s="6"/>
+    </row>
+    <row r="352" spans="2:6">
+      <c r="B352" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="C352" s="5"/>
+      <c r="D352" s="5"/>
+      <c r="E352" s="5"/>
+      <c r="F352" s="6"/>
+    </row>
+    <row r="353" spans="2:6">
+      <c r="B353" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="C353" s="5"/>
+      <c r="D353" s="5"/>
+      <c r="E353" s="5"/>
+      <c r="F353" s="6"/>
+    </row>
+    <row r="354" spans="2:6">
+      <c r="B354" s="4" t="s">
+        <v>985</v>
+      </c>
+      <c r="C354" s="5"/>
+      <c r="D354" s="5"/>
+      <c r="E354" s="5"/>
+      <c r="F354" s="6"/>
+    </row>
+    <row r="355" spans="2:6">
+      <c r="B355" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="C355" s="5"/>
+      <c r="D355" s="5"/>
+      <c r="E355" s="5"/>
+      <c r="F355" s="6"/>
+    </row>
+    <row r="356" spans="2:6">
+      <c r="B356" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C356" s="5"/>
+      <c r="D356" s="5"/>
+      <c r="E356" s="5"/>
+      <c r="F356" s="6"/>
+    </row>
+    <row r="357" spans="2:6" ht="15.75" thickBot="1">
+      <c r="B357" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C357" s="8"/>
+      <c r="D357" s="8"/>
+      <c r="E357" s="8"/>
+      <c r="F357" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>